<commit_message>
delete unused images, modify invoice template,add warranty page
</commit_message>
<xml_diff>
--- a/storage/app/xlsx/invoices.xlsx
+++ b/storage/app/xlsx/invoices.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crosslimits-laravel\storage\app\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77987AA7-F1E9-4017-A4AC-C51F8154635B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC0D60A-61EB-421C-9BFE-0C4880D0CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVOICE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Invoice No.</t>
   </si>
@@ -63,28 +70,59 @@
     <t>Proforma Invoice</t>
   </si>
   <si>
-    <t>Crosslimits ltd</t>
+    <t>Your contact at Crosslimits</t>
   </si>
   <si>
-    <t>*****************</t>
+    <t>Guangzhou，China</t>
   </si>
   <si>
-    <t>*************************</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Reg No.:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 91330782MA28D6BA7K</t>
+    </r>
   </si>
   <si>
-    <t>Tax ID. **************</t>
+    <t>No.222,Xingmin Road,Tianhe district</t>
   </si>
   <si>
-    <t>Registration No. ***********</t>
+    <t>zara@crosslimitsgear.com</t>
   </si>
   <si>
-    <t>zara@crosslimits.com</t>
+    <t>086-18620894001</t>
   </si>
   <si>
-    <t>0086 188888888888</t>
-  </si>
-  <si>
-    <t>Your contact at Crosslimits</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: 38F， Top Plaza C1-Building</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -94,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -138,6 +176,26 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -223,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -241,16 +299,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -273,9 +325,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -495,20 +560,23 @@
   <dimension ref="B1:O996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.69921875" customWidth="1"/>
     <col min="2" max="2" width="4.19921875" customWidth="1"/>
-    <col min="3" max="7" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
     <col min="8" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="20.09765625" customWidth="1"/>
     <col min="11" max="11" width="10.796875" customWidth="1"/>
     <col min="12" max="12" width="13.19921875" customWidth="1"/>
     <col min="13" max="13" width="11.69921875" customWidth="1"/>
-    <col min="14" max="14" width="25.5" customWidth="1"/>
+    <col min="14" max="14" width="32.3984375" customWidth="1"/>
     <col min="15" max="15" width="5.796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,16 +615,16 @@
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B4" s="5"/>
-      <c r="C4" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="26" t="s">
+        <v>10</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -614,9 +682,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="N7" s="22"/>
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -624,8 +690,8 @@
       <c r="C8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
         <v>3</v>
@@ -636,8 +702,8 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="14" t="s">
-        <v>12</v>
+      <c r="N8" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="O8" s="7"/>
     </row>
@@ -656,15 +722,15 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="14" t="s">
-        <v>13</v>
+      <c r="N9" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="O9" s="7"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -678,8 +744,8 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="14" t="s">
-        <v>14</v>
+      <c r="N10" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="O10" s="7"/>
     </row>
@@ -688,10 +754,10 @@
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="23" t="s">
-        <v>16</v>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
       </c>
+      <c r="E11" s="24"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -702,8 +768,8 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="14" t="s">
-        <v>15</v>
+      <c r="N11" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="O11" s="7"/>
     </row>
@@ -713,8 +779,8 @@
         <v>8</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="14" t="s">
-        <v>17</v>
+      <c r="E12" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
@@ -811,8 +877,8 @@
     </row>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="9"/>
       <c r="F18" s="6"/>
       <c r="G18" s="9"/>
@@ -820,8 +886,8 @@
       <c r="I18" s="9"/>
       <c r="J18" s="6"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="18"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
       <c r="N18" s="6"/>
       <c r="O18" s="7"/>
     </row>
@@ -836,8 +902,8 @@
       <c r="I19" s="9"/>
       <c r="J19" s="6"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="19"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="17"/>
       <c r="N19" s="6"/>
       <c r="O19" s="7"/>
     </row>
@@ -852,8 +918,8 @@
       <c r="I20" s="9"/>
       <c r="J20" s="6"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="19"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="17"/>
       <c r="N20" s="6"/>
       <c r="O20" s="7"/>
     </row>
@@ -868,15 +934,15 @@
       <c r="I21" s="9"/>
       <c r="J21" s="6"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="19"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="17"/>
       <c r="N21" s="6"/>
       <c r="O21" s="7"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="20"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="21"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="9"/>
       <c r="F22" s="6"/>
       <c r="G22" s="9"/>
@@ -887,12 +953,12 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="7"/>
-      <c r="O22" s="20"/>
+      <c r="O22" s="18"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="9"/>
       <c r="F23" s="6"/>
       <c r="G23" s="9"/>
@@ -901,14 +967,14 @@
       <c r="J23" s="6"/>
       <c r="K23" s="9"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="22"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="7"/>
       <c r="O23" s="9"/>
     </row>
     <row r="24" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="22"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -917,7 +983,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="22"/>
+      <c r="M24" s="20"/>
       <c r="N24" s="7"/>
       <c r="O24" s="9"/>
     </row>
@@ -959,7 +1025,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="22"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2352,10 +2418,14 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D11:E11"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{0E731400-786F-4522-846F-E828597F21A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add delete button, update invoice template
</commit_message>
<xml_diff>
--- a/storage/app/xlsx/invoices.xlsx
+++ b/storage/app/xlsx/invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crosslimits-laravel\storage\app\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC0D60A-61EB-421C-9BFE-0C4880D0CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D784A65-6D9C-44EF-909D-8AEDDA307F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Invoice No.</t>
   </si>
@@ -76,26 +76,6 @@
     <t>Guangzhou，China</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Reg No.:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> 91330782MA28D6BA7K</t>
-    </r>
-  </si>
-  <si>
     <t>No.222,Xingmin Road,Tianhe district</t>
   </si>
   <si>
@@ -105,24 +85,16 @@
     <t>086-18620894001</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Add</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>: 38F， Top Plaza C1-Building</t>
-    </r>
+    <t>38F， Top Plaza C1-Building</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>91330782MA28D6BA7K</t>
+  </si>
+  <si>
+    <t>Registration No.:</t>
   </si>
 </sst>
 </file>
@@ -281,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -334,13 +306,14 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -559,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -575,7 +548,7 @@
     <col min="10" max="10" width="20.09765625" customWidth="1"/>
     <col min="11" max="11" width="10.796875" customWidth="1"/>
     <col min="12" max="12" width="13.19921875" customWidth="1"/>
-    <col min="13" max="13" width="11.69921875" customWidth="1"/>
+    <col min="13" max="13" width="15.19921875" customWidth="1"/>
     <col min="14" max="14" width="32.3984375" customWidth="1"/>
     <col min="15" max="15" width="5.796875" customWidth="1"/>
   </cols>
@@ -622,7 +595,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="24" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="6"/>
@@ -701,9 +674,11 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="23" t="s">
+      <c r="M8" s="27" t="s">
         <v>17</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="O8" s="7"/>
     </row>
@@ -723,7 +698,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O9" s="7"/>
     </row>
@@ -755,9 +730,9 @@
         <v>6</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -767,9 +742,11 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="M11" s="27" t="s">
+        <v>19</v>
+      </c>
       <c r="N11" s="23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O11" s="7"/>
     </row>
@@ -780,7 +757,7 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">

</xml_diff>